<commit_message>
Implementing Clockify REST API.
</commit_message>
<xml_diff>
--- a/src/E3kWorkReports/template.xlsx
+++ b/src/E3kWorkReports/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\Automation\src\E3kWorkReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5FF417-94F8-430F-B3B1-49AD7CF271A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F980A56-7684-42E2-ACEB-263528A4A662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26625" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23390" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boris" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00#"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -102,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -134,12 +133,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -150,6 +143,15 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -503,18 +505,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7265625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="85.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -527,309 +529,276 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="C18" s="9"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="12"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="12"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="12"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="12"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="12"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="12"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="12"/>
+      <c r="E30" s="16"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="12"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="11"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="11"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="11"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="11"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="11"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="11"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="11"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="11"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="11"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="11"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="11"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="11"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="11"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="11"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="11"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="11"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="11"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="11"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F65">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="F1:F1048576">
@@ -846,22 +815,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987C4A3C-EFF0-4B12-BCF8-AF1175EE8DAD}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7265625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="85.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -874,138 +843,119 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="12"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E23" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="F1:F1048576">
@@ -1026,18 +976,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7265625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="85.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Removed Andrej Bratoz from monthly work report.
</commit_message>
<xml_diff>
--- a/src/E3kWorkReports/template.xlsx
+++ b/src/E3kWorkReports/template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\Automation\src\E3kWorkReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F980A56-7684-42E2-ACEB-263528A4A662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF941A3-6342-4B45-ADDF-57B73CE19BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23390" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boris" sheetId="1" r:id="rId1"/>
-    <sheet name="Andrej" sheetId="5" r:id="rId2"/>
-    <sheet name="Borut" sheetId="6" r:id="rId3"/>
+    <sheet name="Borut" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Working code / project</t>
   </si>
@@ -48,9 +47,6 @@
   </si>
   <si>
     <t>Boris Turk</t>
-  </si>
-  <si>
-    <t>Andrej Bratož</t>
   </si>
   <si>
     <t>Borut Kaučič</t>
@@ -159,17 +155,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -802,7 +788,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -813,163 +799,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987C4A3C-EFF0-4B12-BCF8-AF1175EE8DAD}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7265625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="D22" s="1"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
-    <sortCondition ref="A2"/>
-  </sortState>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB4954A-FFD2-4F5B-B6B9-4C0A4D1F89B1}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F1"/>
@@ -989,7 +818,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>

</xml_diff>